<commit_message>
Updated the post-hoc script to remove wilcoxon since it isnt in the paper. Ran it and got results in csv format.
</commit_message>
<xml_diff>
--- a/WekaTesting/output/Results.xlsx
+++ b/WekaTesting/output/Results.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17766"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28410"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\melkiga\Google Drive\Research\Cano\MultiInstanceClassification\WekaTesting\output\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabriellamelki/Documents/Research/MultiInstanceLearning/WekaTesting/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="10215" activeTab="6"/>
+    <workbookView xWindow="1020" yWindow="460" windowWidth="21580" windowHeight="10220" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,9 +20,15 @@
     <sheet name="AUC" sheetId="6" r:id="rId6"/>
     <sheet name="Time" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -185,7 +191,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
@@ -277,7 +283,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="164" formatCode="0.0000"/>
@@ -329,7 +334,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -697,14 +701,14 @@
       <selection activeCell="C89" sqref="C89"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="13.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="8" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>29</v>
       </c>
@@ -730,7 +734,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -756,7 +760,7 @@
         <v>0.67500000000000004</v>
       </c>
     </row>
-    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -782,7 +786,7 @@
         <v>0.63749999999999996</v>
       </c>
     </row>
-    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -808,7 +812,7 @@
         <v>0.6875</v>
       </c>
     </row>
-    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -834,7 +838,7 @@
         <v>0.87919621749408983</v>
       </c>
     </row>
-    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -860,7 +864,7 @@
         <v>0.70430107526881724</v>
       </c>
     </row>
-    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -886,7 +890,7 @@
         <v>0.59394409937888204</v>
       </c>
     </row>
-    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -912,7 +916,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -938,7 +942,7 @@
         <v>0.7653968253968253</v>
       </c>
     </row>
-    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -964,7 +968,7 @@
         <v>0.85688888888888881</v>
       </c>
     </row>
-    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -990,7 +994,7 @@
         <v>0.82495238095238088</v>
       </c>
     </row>
-    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1016,7 +1020,7 @@
         <v>0.77</v>
       </c>
     </row>
-    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -1042,7 +1046,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -1068,7 +1072,7 @@
         <v>0.62</v>
       </c>
     </row>
-    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -1094,7 +1098,7 @@
         <v>0.80304324398438165</v>
       </c>
     </row>
-    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -1120,7 +1124,7 @@
         <v>0.84078817210319867</v>
       </c>
     </row>
-    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>1</v>
       </c>
@@ -1146,7 +1150,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>2</v>
       </c>
@@ -1172,7 +1176,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>3</v>
       </c>
@@ -1198,7 +1202,7 @@
         <v>0.49999999999999994</v>
       </c>
     </row>
-    <row r="20" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>4</v>
       </c>
@@ -1224,7 +1228,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>5</v>
       </c>
@@ -1250,7 +1254,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="22" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>6</v>
       </c>
@@ -1276,7 +1280,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>7</v>
       </c>
@@ -1302,7 +1306,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>8</v>
       </c>
@@ -1328,7 +1332,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>9</v>
       </c>
@@ -1354,7 +1358,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>10</v>
       </c>
@@ -1380,7 +1384,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>11</v>
       </c>
@@ -1406,7 +1410,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="28" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>12</v>
       </c>
@@ -1432,7 +1436,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>13</v>
       </c>
@@ -1458,7 +1462,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="30" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>14</v>
       </c>
@@ -1484,7 +1488,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="31" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>15</v>
       </c>
@@ -1510,7 +1514,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="32" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>1</v>
       </c>
@@ -1536,7 +1540,7 @@
         <v>0.42500000000000004</v>
       </c>
     </row>
-    <row r="33" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>2</v>
       </c>
@@ -1562,7 +1566,7 @@
         <v>0.61250000000000004</v>
       </c>
     </row>
-    <row r="34" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>3</v>
       </c>
@@ -1588,7 +1592,7 @@
         <v>0.44999999999999996</v>
       </c>
     </row>
-    <row r="35" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>4</v>
       </c>
@@ -1614,7 +1618,7 @@
         <v>0.87966903073286062</v>
       </c>
     </row>
-    <row r="36" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>5</v>
       </c>
@@ -1640,7 +1644,7 @@
         <v>0.6980976013234077</v>
       </c>
     </row>
-    <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>6</v>
       </c>
@@ -1666,7 +1670,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="38" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>7</v>
       </c>
@@ -1692,7 +1696,7 @@
         <v>0.69321428571428567</v>
       </c>
     </row>
-    <row r="39" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>8</v>
       </c>
@@ -1718,7 +1722,7 @@
         <v>0.6186031746031746</v>
       </c>
     </row>
-    <row r="40" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>9</v>
       </c>
@@ -1744,7 +1748,7 @@
         <v>0.6980952380952381</v>
       </c>
     </row>
-    <row r="41" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>10</v>
       </c>
@@ -1770,7 +1774,7 @@
         <v>0.72571428571428576</v>
       </c>
     </row>
-    <row r="42" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>11</v>
       </c>
@@ -1796,7 +1800,7 @@
         <v>0.71</v>
       </c>
     </row>
-    <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>12</v>
       </c>
@@ -1822,7 +1826,7 @@
         <v>0.79</v>
       </c>
     </row>
-    <row r="44" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>13</v>
       </c>
@@ -1848,7 +1852,7 @@
         <v>0.58000000000000007</v>
       </c>
     </row>
-    <row r="45" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>14</v>
       </c>
@@ -1874,7 +1878,7 @@
         <v>0.60331632987238226</v>
       </c>
     </row>
-    <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>15</v>
       </c>
@@ -1900,7 +1904,7 @@
         <v>0.6014583079526068</v>
       </c>
     </row>
-    <row r="47" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
         <v>1</v>
       </c>
@@ -1926,7 +1930,7 @@
         <v>0.72499999999999998</v>
       </c>
     </row>
-    <row r="48" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>2</v>
       </c>
@@ -1952,7 +1956,7 @@
         <v>0.72499999999999998</v>
       </c>
     </row>
-    <row r="49" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>3</v>
       </c>
@@ -1978,7 +1982,7 @@
         <v>0.37499999999999994</v>
       </c>
     </row>
-    <row r="50" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
         <v>4</v>
       </c>
@@ -2004,7 +2008,7 @@
         <v>0.76761229314420798</v>
       </c>
     </row>
-    <row r="51" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
         <v>5</v>
       </c>
@@ -2030,7 +2034,7 @@
         <v>0.7431761786600497</v>
       </c>
     </row>
-    <row r="52" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
         <v>6</v>
       </c>
@@ -2056,7 +2060,7 @@
         <v>0.50957556935817805</v>
       </c>
     </row>
-    <row r="53" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
         <v>7</v>
       </c>
@@ -2082,7 +2086,7 @@
         <v>0.73916666666666675</v>
       </c>
     </row>
-    <row r="54" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
         <v>8</v>
       </c>
@@ -2108,7 +2112,7 @@
         <v>0.58241269841269838</v>
       </c>
     </row>
-    <row r="55" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
         <v>9</v>
       </c>
@@ -2134,7 +2138,7 @@
         <v>0.65777777777777779</v>
       </c>
     </row>
-    <row r="56" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
         <v>10</v>
       </c>
@@ -2160,7 +2164,7 @@
         <v>0.61422222222222222</v>
       </c>
     </row>
-    <row r="57" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
         <v>11</v>
       </c>
@@ -2186,7 +2190,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="58" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
         <v>12</v>
       </c>
@@ -2212,7 +2216,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="59" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
         <v>13</v>
       </c>
@@ -2238,7 +2242,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="60" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
         <v>14</v>
       </c>
@@ -2264,7 +2268,7 @@
         <v>0.55363426053284504</v>
       </c>
     </row>
-    <row r="61" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
         <v>15</v>
       </c>
@@ -2290,7 +2294,7 @@
         <v>0.52979669861619971</v>
       </c>
     </row>
-    <row r="62" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" s="2">
         <v>1</v>
       </c>
@@ -2316,7 +2320,7 @@
         <v>0.72499999999999998</v>
       </c>
     </row>
-    <row r="63" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" s="2">
         <v>2</v>
       </c>
@@ -2342,7 +2346,7 @@
         <v>0.71249999999999991</v>
       </c>
     </row>
-    <row r="64" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" s="2">
         <v>3</v>
       </c>
@@ -2368,7 +2372,7 @@
         <v>0.73750000000000004</v>
       </c>
     </row>
-    <row r="65" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" s="2">
         <v>4</v>
       </c>
@@ -2394,7 +2398,7 @@
         <v>0.78156028368794328</v>
       </c>
     </row>
-    <row r="66" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" s="2">
         <v>5</v>
       </c>
@@ -2420,7 +2424,7 @@
         <v>0.67721257237386268</v>
       </c>
     </row>
-    <row r="67" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" s="2">
         <v>6</v>
       </c>
@@ -2446,7 +2450,7 @@
         <v>0.71842650103519667</v>
       </c>
     </row>
-    <row r="68" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" s="2">
         <v>7</v>
       </c>
@@ -2472,7 +2476,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="69" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" s="2">
         <v>8</v>
       </c>
@@ -2498,7 +2502,7 @@
         <v>0.64203174603174606</v>
       </c>
     </row>
-    <row r="70" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" s="2">
         <v>9</v>
       </c>
@@ -2524,7 +2528,7 @@
         <v>0.78501587301587306</v>
       </c>
     </row>
-    <row r="71" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" s="2">
         <v>10</v>
       </c>
@@ -2550,7 +2554,7 @@
         <v>0.80514285714285716</v>
       </c>
     </row>
-    <row r="72" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" s="2">
         <v>11</v>
       </c>
@@ -2576,7 +2580,7 @@
         <v>0.72</v>
       </c>
     </row>
-    <row r="73" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" s="2">
         <v>12</v>
       </c>
@@ -2602,7 +2606,7 @@
         <v>0.81</v>
       </c>
     </row>
-    <row r="74" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" s="2">
         <v>13</v>
       </c>
@@ -2628,7 +2632,7 @@
         <v>0.52500000000000002</v>
       </c>
     </row>
-    <row r="75" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" s="2">
         <v>14</v>
       </c>
@@ -2654,7 +2658,7 @@
         <v>0.62717925071240743</v>
       </c>
     </row>
-    <row r="76" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" s="2">
         <v>15</v>
       </c>
@@ -2680,7 +2684,7 @@
         <v>0.63912134629251682</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" s="2">
         <v>1</v>
       </c>
@@ -2706,7 +2710,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" s="2">
         <v>2</v>
       </c>
@@ -2732,7 +2736,7 @@
         <v>0.63749999999999996</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" s="2">
         <v>3</v>
       </c>
@@ -2758,7 +2762,7 @@
         <v>0.46250000000000002</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" s="2">
         <v>4</v>
       </c>
@@ -2784,7 +2788,7 @@
         <v>0.80189125295508279</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" s="2">
         <v>5</v>
       </c>
@@ -2810,7 +2814,7 @@
         <v>0.69003308519437545</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" s="2">
         <v>6</v>
       </c>
@@ -2836,7 +2840,7 @@
         <v>0.80978260869565211</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" s="2">
         <v>7</v>
       </c>
@@ -2862,7 +2866,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84" s="2">
         <v>8</v>
       </c>
@@ -2888,7 +2892,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" s="2">
         <v>9</v>
       </c>
@@ -2914,7 +2918,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" s="2">
         <v>10</v>
       </c>
@@ -2940,7 +2944,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" s="2">
         <v>11</v>
       </c>
@@ -2966,7 +2970,7 @@
         <v>0.755</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" s="2">
         <v>12</v>
       </c>
@@ -2992,7 +2996,7 @@
         <v>0.79999999999999993</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" s="2">
         <v>13</v>
       </c>
@@ -3018,7 +3022,7 @@
         <v>0.59</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90" s="2">
         <v>14</v>
       </c>
@@ -3044,7 +3048,7 @@
         <v>0.52009456264775411</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" s="2">
         <v>15</v>
       </c>
@@ -3070,7 +3074,7 @@
         <v>0.52677547099964861</v>
       </c>
     </row>
-    <row r="92" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92" s="2">
         <v>1</v>
       </c>
@@ -3096,7 +3100,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="93" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93" s="2">
         <v>2</v>
       </c>
@@ -3122,7 +3126,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="94" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" s="2">
         <v>3</v>
       </c>
@@ -3148,7 +3152,7 @@
         <v>0.49999999999999994</v>
       </c>
     </row>
-    <row r="95" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" s="2">
         <v>4</v>
       </c>
@@ -3174,7 +3178,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="96" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96" s="2">
         <v>5</v>
       </c>
@@ -3200,7 +3204,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="97" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" s="2">
         <v>6</v>
       </c>
@@ -3226,7 +3230,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="98" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98" s="2">
         <v>7</v>
       </c>
@@ -3252,7 +3256,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="99" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99" s="2">
         <v>8</v>
       </c>
@@ -3278,7 +3282,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="100" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100" s="2">
         <v>9</v>
       </c>
@@ -3304,7 +3308,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="101" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101" s="2">
         <v>10</v>
       </c>
@@ -3330,7 +3334,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="102" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102" s="2">
         <v>11</v>
       </c>
@@ -3356,7 +3360,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="103" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103" s="2">
         <v>12</v>
       </c>
@@ -3382,7 +3386,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="104" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" s="2">
         <v>13</v>
       </c>
@@ -3408,7 +3412,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="105" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" s="2">
         <v>14</v>
       </c>
@@ -3434,7 +3438,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="106" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" s="2">
         <v>15</v>
       </c>
@@ -3460,7 +3464,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="107" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107" s="2">
         <v>1</v>
       </c>
@@ -3486,7 +3490,7 @@
         <v>0.2142857142857143</v>
       </c>
     </row>
-    <row r="108" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108" s="2">
         <v>2</v>
       </c>
@@ -3512,7 +3516,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="109" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109" s="2">
         <v>3</v>
       </c>
@@ -3538,7 +3542,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="110" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A110" s="2">
         <v>4</v>
       </c>
@@ -3564,7 +3568,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="111" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111" s="2">
         <v>5</v>
       </c>
@@ -3590,7 +3594,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="112" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A112" s="2">
         <v>6</v>
       </c>
@@ -3616,7 +3620,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="113" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A113" s="2">
         <v>7</v>
       </c>
@@ -3642,7 +3646,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="114" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A114" s="2">
         <v>8</v>
       </c>
@@ -3668,7 +3672,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="115" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A115" s="2">
         <v>9</v>
       </c>
@@ -3694,7 +3698,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="116" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A116" s="2">
         <v>10</v>
       </c>
@@ -3720,7 +3724,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="117" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A117" s="2">
         <v>11</v>
       </c>
@@ -3746,7 +3750,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="118" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A118" s="2">
         <v>12</v>
       </c>
@@ -3772,7 +3776,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="119" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A119" s="2">
         <v>13</v>
       </c>
@@ -3798,7 +3802,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="120" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120" s="2">
         <v>14</v>
       </c>
@@ -3824,7 +3828,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="121" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A121" s="2">
         <v>15</v>
       </c>
@@ -3850,7 +3854,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="122" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A122" s="2">
         <v>1</v>
       </c>
@@ -3876,7 +3880,7 @@
         <v>0.68110000000000004</v>
       </c>
     </row>
-    <row r="123" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A123" s="2">
         <v>2</v>
       </c>
@@ -3902,7 +3906,7 @@
         <v>0.44999999999999996</v>
       </c>
     </row>
-    <row r="124" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A124" s="2">
         <v>3</v>
       </c>
@@ -3928,7 +3932,7 @@
         <v>0.63749999999999996</v>
       </c>
     </row>
-    <row r="125" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A125" s="2">
         <v>4</v>
       </c>
@@ -3954,7 +3958,7 @@
         <v>0.85886524822695032</v>
       </c>
     </row>
-    <row r="126" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A126" s="2">
         <v>5</v>
       </c>
@@ -3980,7 +3984,7 @@
         <v>0.64350703060380476</v>
       </c>
     </row>
-    <row r="127" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A127" s="2">
         <v>6</v>
       </c>
@@ -4006,7 +4010,7 @@
         <v>0.60481366459627317</v>
       </c>
     </row>
-    <row r="128" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A128" s="2">
         <v>7</v>
       </c>
@@ -4032,7 +4036,7 @@
         <v>0.62809523809523815</v>
       </c>
     </row>
-    <row r="129" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A129" s="2">
         <v>8</v>
       </c>
@@ -4058,7 +4062,7 @@
         <v>0.71371428571428575</v>
       </c>
     </row>
-    <row r="130" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A130" s="2">
         <v>9</v>
       </c>
@@ -4084,7 +4088,7 @@
         <v>0.82114285714285717</v>
       </c>
     </row>
-    <row r="131" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A131" s="2">
         <v>10</v>
       </c>
@@ -4110,7 +4114,7 @@
         <v>0.81301587301587297</v>
       </c>
     </row>
-    <row r="132" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A132" s="2">
         <v>11</v>
       </c>
@@ -4136,7 +4140,7 @@
         <v>0.72499999999999998</v>
       </c>
     </row>
-    <row r="133" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A133" s="2">
         <v>12</v>
       </c>
@@ -4162,7 +4166,7 @@
         <v>0.82499999999999996</v>
       </c>
     </row>
-    <row r="134" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A134" s="2">
         <v>13</v>
       </c>
@@ -4188,7 +4192,7 @@
         <v>0.64999999999999991</v>
       </c>
     </row>
-    <row r="135" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A135" s="2">
         <v>14</v>
       </c>
@@ -4214,7 +4218,7 @@
         <v>0.80810367307942554</v>
       </c>
     </row>
-    <row r="136" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A136" s="2">
         <v>15</v>
       </c>
@@ -4240,7 +4244,7 @@
         <v>0.84344485800982805</v>
       </c>
     </row>
-    <row r="137" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A137" s="2">
         <v>1</v>
       </c>
@@ -4266,7 +4270,7 @@
         <v>0.69047619047619047</v>
       </c>
     </row>
-    <row r="138" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A138" s="2">
         <v>2</v>
       </c>
@@ -4292,7 +4296,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="139" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A139" s="2">
         <v>3</v>
       </c>
@@ -4318,7 +4322,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="140" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A140" s="2">
         <v>4</v>
       </c>
@@ -4344,7 +4348,7 @@
         <v>0.85886524822695032</v>
       </c>
     </row>
-    <row r="141" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A141" s="2">
         <v>5</v>
       </c>
@@ -4370,7 +4374,7 @@
         <v>0.63172043010752688</v>
       </c>
     </row>
-    <row r="142" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A142" s="2">
         <v>6</v>
       </c>
@@ -4396,7 +4400,7 @@
         <v>0.6837474120082816</v>
       </c>
     </row>
-    <row r="143" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A143" s="2">
         <v>7</v>
       </c>
@@ -4422,7 +4426,7 @@
         <v>0.67321428571428577</v>
       </c>
     </row>
-    <row r="144" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A144" s="2">
         <v>8</v>
       </c>
@@ -4448,7 +4452,7 @@
         <v>0.72571428571428576</v>
       </c>
     </row>
-    <row r="145" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A145" s="2">
         <v>9</v>
       </c>
@@ -4474,7 +4478,7 @@
         <v>0.80120634920634914</v>
       </c>
     </row>
-    <row r="146" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A146" s="2">
         <v>10</v>
       </c>
@@ -4500,7 +4504,7 @@
         <v>0.81701587301587297</v>
       </c>
     </row>
-    <row r="147" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A147" s="2">
         <v>11</v>
       </c>
@@ -4526,7 +4530,7 @@
         <v>0.66500000000000004</v>
       </c>
     </row>
-    <row r="148" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A148" s="2">
         <v>12</v>
       </c>
@@ -4552,7 +4556,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="149" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A149" s="2">
         <v>13</v>
       </c>
@@ -4578,7 +4582,7 @@
         <v>0.64500000000000002</v>
       </c>
     </row>
-    <row r="150" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A150" s="2">
         <v>14</v>
       </c>
@@ -4604,7 +4608,7 @@
         <v>0.8122776865162642</v>
       </c>
     </row>
-    <row r="151" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A151" s="2">
         <v>15</v>
       </c>
@@ -4644,25 +4648,25 @@
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -4700,12 +4704,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>24</v>
       </c>
       <c r="B2" s="5">
-        <v>0.6</v>
+        <v>0.7</v>
       </c>
       <c r="C2">
         <v>0.5</v>
@@ -4738,7 +4742,7 @@
         <v>0.75639999999999996</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -4776,12 +4780,12 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>28</v>
       </c>
       <c r="B4" s="5">
-        <v>0.65</v>
+        <v>0.7</v>
       </c>
       <c r="C4">
         <v>0.5</v>
@@ -4814,7 +4818,7 @@
         <v>0.63749999999999996</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -4852,7 +4856,7 @@
         <v>0.85870000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -4890,7 +4894,7 @@
         <v>0.67330000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -4928,7 +4932,7 @@
         <v>0.80530000000000002</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -4966,7 +4970,7 @@
         <v>0.88600000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -5004,7 +5008,7 @@
         <v>0.76060000000000005</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -5042,7 +5046,7 @@
         <v>0.85640000000000005</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -5080,7 +5084,7 @@
         <v>0.83509999999999995</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -5118,7 +5122,7 @@
         <v>0.72499999999999998</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -5156,7 +5160,7 @@
         <v>0.82499999999999996</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -5194,7 +5198,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -5232,7 +5236,7 @@
         <v>0.9355</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -5280,15 +5284,15 @@
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -5326,12 +5330,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>24</v>
       </c>
       <c r="B2" s="6">
-        <v>0.63849999999999996</v>
+        <v>0.63829999999999998</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -5364,7 +5368,7 @@
         <v>0.71160000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -5402,12 +5406,12 @@
         <v>0.44440000000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>28</v>
       </c>
       <c r="B4" s="6">
-        <v>0.63</v>
+        <v>0.67</v>
       </c>
       <c r="C4">
         <v>0.5</v>
@@ -5440,7 +5444,7 @@
         <v>0.6038</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -5478,7 +5482,7 @@
         <v>0.8478</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -5516,7 +5520,7 @@
         <v>0.71640000000000004</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -5554,7 +5558,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -5592,7 +5596,7 @@
         <v>0.90110000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -5630,7 +5634,7 @@
         <v>0.66669999999999996</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -5668,7 +5672,7 @@
         <v>0.83330000000000004</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -5706,7 +5710,7 @@
         <v>0.7581</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -5744,7 +5748,7 @@
         <v>0.73199999999999998</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -5782,7 +5786,7 @@
         <v>0.82830000000000004</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -5820,7 +5824,7 @@
         <v>0.67049999999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -5858,7 +5862,7 @@
         <v>0.94489999999999996</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -5906,15 +5910,15 @@
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -5952,7 +5956,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -5990,7 +5994,7 @@
         <v>0.91249999999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -6028,12 +6032,12 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>28</v>
       </c>
       <c r="B4" s="7">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="C4">
         <v>0.9</v>
@@ -6066,7 +6070,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -6104,7 +6108,7 @@
         <v>0.86670000000000003</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -6142,7 +6146,7 @@
         <v>0.7742</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -6180,7 +6184,7 @@
         <v>0.92390000000000005</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -6218,7 +6222,7 @@
         <v>0.97619999999999996</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -6256,7 +6260,7 @@
         <v>0.57140000000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -6294,7 +6298,7 @@
         <v>0.71430000000000005</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -6332,7 +6336,7 @@
         <v>0.746</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -6370,7 +6374,7 @@
         <v>0.71</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -6408,7 +6412,7 @@
         <v>0.82</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -6446,7 +6450,7 @@
         <v>0.59</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -6484,7 +6488,7 @@
         <v>0.98260000000000003</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -6532,18 +6536,18 @@
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -6581,7 +6585,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -6619,7 +6623,7 @@
         <v>0.5121</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -6657,12 +6661,12 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>28</v>
       </c>
       <c r="B4" s="9">
-        <v>0.35</v>
+        <v>0.4</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -6695,7 +6699,7 @@
         <v>0.27500000000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -6733,7 +6737,7 @@
         <v>0.71740000000000004</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -6771,7 +6775,7 @@
         <v>0.29399999999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -6809,7 +6813,7 @@
         <v>0.24579999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -6847,7 +6851,7 @@
         <v>0.33639999999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -6885,7 +6889,7 @@
         <v>0.44309999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -6923,7 +6927,7 @@
         <v>0.66590000000000005</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -6961,7 +6965,7 @@
         <v>0.62849999999999995</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -6999,7 +7003,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -7037,7 +7041,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -7075,7 +7079,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -7113,7 +7117,7 @@
         <v>0.69059999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -7160,17 +7164,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -7208,12 +7212,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>24</v>
       </c>
       <c r="B2" s="7">
-        <v>0.5</v>
+        <v>0.67</v>
       </c>
       <c r="C2">
         <v>0.5</v>
@@ -7246,7 +7250,7 @@
         <v>0.68110000000000004</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -7284,12 +7288,12 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>28</v>
       </c>
       <c r="B4" s="7">
-        <v>0.65</v>
+        <v>0.7</v>
       </c>
       <c r="C4">
         <v>0.5</v>
@@ -7322,7 +7326,7 @@
         <v>0.63749999999999996</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -7360,7 +7364,7 @@
         <v>0.8589</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -7398,7 +7402,7 @@
         <v>0.64349999999999996</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -7436,7 +7440,7 @@
         <v>0.6048</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -7474,7 +7478,7 @@
         <v>0.62809999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -7512,7 +7516,7 @@
         <v>0.7137</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -7550,7 +7554,7 @@
         <v>0.82110000000000005</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -7588,7 +7592,7 @@
         <v>0.81299999999999994</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -7626,7 +7630,7 @@
         <v>0.72499999999999998</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -7664,7 +7668,7 @@
         <v>0.82499999999999996</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -7702,7 +7706,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -7740,7 +7744,7 @@
         <v>0.80810000000000004</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -7787,25 +7791,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" customWidth="1"/>
-    <col min="7" max="7" width="9.5703125" customWidth="1"/>
-    <col min="8" max="8" width="9.42578125" customWidth="1"/>
-    <col min="9" max="9" width="11.5703125" customWidth="1"/>
+    <col min="2" max="3" width="10.5" customWidth="1"/>
+    <col min="4" max="4" width="15.83203125" customWidth="1"/>
+    <col min="6" max="6" width="13.1640625" customWidth="1"/>
+    <col min="7" max="8" width="9.5" customWidth="1"/>
+    <col min="9" max="9" width="11.5" customWidth="1"/>
     <col min="11" max="11" width="10" customWidth="1"/>
-    <col min="12" max="12" width="10.42578125" customWidth="1"/>
+    <col min="12" max="12" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -7843,7 +7845,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>45</v>
       </c>
@@ -7881,7 +7883,7 @@
         <v>1084.95</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -7919,7 +7921,7 @@
         <v>15.25</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -7957,7 +7959,7 @@
         <v>10.76</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>40</v>
       </c>
@@ -7995,7 +7997,7 @@
         <v>759.45</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>41</v>
       </c>
@@ -8033,7 +8035,7 @@
         <v>16759.05</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>48</v>
       </c>
@@ -8071,7 +8073,7 @@
         <v>10.75</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>47</v>
       </c>
@@ -8109,7 +8111,7 @@
         <v>592948.94999999995</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>42</v>
       </c>
@@ -8147,7 +8149,7 @@
         <v>153.9</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>43</v>
       </c>
@@ -8185,7 +8187,7 @@
         <v>853.15</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>44</v>
       </c>
@@ -8223,7 +8225,7 @@
         <v>1618.95</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>46</v>
       </c>
@@ -8261,7 +8263,7 @@
         <v>11927.9</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>37</v>
       </c>
@@ -8299,7 +8301,7 @@
         <v>1462.2</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>38</v>
       </c>
@@ -8337,7 +8339,7 @@
         <v>1729.1</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>35</v>
       </c>
@@ -8375,7 +8377,7 @@
         <v>79149.75</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>39</v>
       </c>

</xml_diff>

<commit_message>
Updated results for new Musk2 results
</commit_message>
<xml_diff>
--- a/WekaTesting/output/Results.xlsx
+++ b/WekaTesting/output/Results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1020" yWindow="460" windowWidth="21580" windowHeight="10220" activeTab="5"/>
+    <workbookView xWindow="3360" yWindow="2640" windowWidth="21580" windowHeight="10220" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -4648,7 +4648,7 @@
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4861,7 +4861,7 @@
         <v>20</v>
       </c>
       <c r="B6" s="5">
-        <v>0.81459999999999999</v>
+        <v>0.82179999999999997</v>
       </c>
       <c r="C6">
         <v>0.6139</v>
@@ -5284,7 +5284,7 @@
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5910,7 +5910,7 @@
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6536,7 +6536,7 @@
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6742,7 +6742,7 @@
         <v>20</v>
       </c>
       <c r="B6" s="9">
-        <v>0.62629999999999997</v>
+        <v>0.65400000000000003</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -7165,7 +7165,7 @@
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7369,7 +7369,7 @@
         <v>20</v>
       </c>
       <c r="B6" s="7">
-        <v>0.83509999999999995</v>
+        <v>0.84060000000000001</v>
       </c>
       <c r="C6">
         <v>0.5</v>

</xml_diff>

<commit_message>
Updated precision and recall for MIRSVM musk2
</commit_message>
<xml_diff>
--- a/WekaTesting/output/Results.xlsx
+++ b/WekaTesting/output/Results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3360" yWindow="2640" windowWidth="21580" windowHeight="10220" activeTab="5"/>
+    <workbookView xWindow="3360" yWindow="2640" windowWidth="21580" windowHeight="10220" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -5284,7 +5284,7 @@
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5487,7 +5487,7 @@
         <v>20</v>
       </c>
       <c r="B6" s="6">
-        <v>0.7167</v>
+        <v>0.70589999999999997</v>
       </c>
       <c r="C6">
         <v>0.6139</v>
@@ -5909,8 +5909,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6113,7 +6113,7 @@
         <v>20</v>
       </c>
       <c r="B6" s="7">
-        <v>0.92500000000000004</v>
+        <v>0.92310000000000003</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -7164,7 +7164,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated new results for suramin
</commit_message>
<xml_diff>
--- a/WekaTesting/output/Results.xlsx
+++ b/WekaTesting/output/Results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3360" yWindow="2640" windowWidth="21580" windowHeight="10220" activeTab="3"/>
+    <workbookView xWindow="3660" yWindow="1800" windowWidth="21580" windowHeight="10220" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -4648,7 +4648,7 @@
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4709,7 +4709,7 @@
         <v>24</v>
       </c>
       <c r="B2" s="5">
-        <v>0.7</v>
+        <v>0.84619999999999995</v>
       </c>
       <c r="C2">
         <v>0.5</v>
@@ -5284,7 +5284,7 @@
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5335,7 +5335,7 @@
         <v>24</v>
       </c>
       <c r="B2" s="6">
-        <v>0.63829999999999998</v>
+        <v>0.77780000000000005</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -5909,8 +5909,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6536,7 +6536,7 @@
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6590,7 +6590,7 @@
         <v>24</v>
       </c>
       <c r="B2" s="8">
-        <v>0.63200000000000001</v>
+        <v>0.68289999999999995</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -7164,8 +7164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7217,7 +7217,7 @@
         <v>24</v>
       </c>
       <c r="B2" s="7">
-        <v>0.67</v>
+        <v>0.83330000000000004</v>
       </c>
       <c r="C2">
         <v>0.5</v>

</xml_diff>

<commit_message>
Updated results for MIRSVM and plugged them into Results
Added parameters for getting those results
</commit_message>
<xml_diff>
--- a/WekaTesting/output/Results.xlsx
+++ b/WekaTesting/output/Results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3660" yWindow="1800" windowWidth="21580" windowHeight="10220" activeTab="5"/>
+    <workbookView xWindow="2660" yWindow="1780" windowWidth="21580" windowHeight="10220" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -4648,7 +4648,7 @@
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4785,7 +4785,7 @@
         <v>28</v>
       </c>
       <c r="B4" s="5">
-        <v>0.7</v>
+        <v>0.75</v>
       </c>
       <c r="C4">
         <v>0.5</v>
@@ -4937,7 +4937,7 @@
         <v>26</v>
       </c>
       <c r="B8" s="5">
-        <v>0.88249999999999995</v>
+        <v>0.88600000000000001</v>
       </c>
       <c r="C8">
         <v>0.87050000000000005</v>
@@ -5284,7 +5284,7 @@
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5411,7 +5411,7 @@
         <v>28</v>
       </c>
       <c r="B4" s="6">
-        <v>0.67</v>
+        <v>0.72719999999999996</v>
       </c>
       <c r="C4">
         <v>0.5</v>
@@ -5563,7 +5563,7 @@
         <v>26</v>
       </c>
       <c r="B8" s="6">
-        <v>0.65</v>
+        <v>1</v>
       </c>
       <c r="C8">
         <v>0.87050000000000005</v>
@@ -5910,7 +5910,7 @@
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6536,7 +6536,7 @@
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6666,7 +6666,7 @@
         <v>28</v>
       </c>
       <c r="B4" s="9">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -6818,7 +6818,7 @@
         <v>26</v>
       </c>
       <c r="B8" s="9">
-        <v>0.45419999999999999</v>
+        <v>0.21</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -7165,7 +7165,7 @@
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7293,7 +7293,7 @@
         <v>28</v>
       </c>
       <c r="B4" s="7">
-        <v>0.7</v>
+        <v>0.75</v>
       </c>
       <c r="C4">
         <v>0.5</v>
@@ -7445,7 +7445,7 @@
         <v>26</v>
       </c>
       <c r="B8" s="7">
-        <v>0.72430000000000005</v>
+        <v>0.65</v>
       </c>
       <c r="C8">
         <v>0.5</v>

</xml_diff>

<commit_message>
Updated results (suramin was wrong)
</commit_message>
<xml_diff>
--- a/WekaTesting/output/Results.xlsx
+++ b/WekaTesting/output/Results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2660" yWindow="1780" windowWidth="21580" windowHeight="10220" activeTab="5"/>
+    <workbookView xWindow="2660" yWindow="1780" windowWidth="21580" windowHeight="10220" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -4647,8 +4647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4709,7 +4709,7 @@
         <v>24</v>
       </c>
       <c r="B2" s="5">
-        <v>0.84619999999999995</v>
+        <v>0.8</v>
       </c>
       <c r="C2">
         <v>0.5</v>
@@ -5284,7 +5284,7 @@
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7164,8 +7164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>